<commit_message>
A set of testing files and a  description of use scenarios.
</commit_message>
<xml_diff>
--- a/inst/as_limity.xlsx
+++ b/inst/as_limity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zajac/Dropbox/PEJK/ASIA/Pakiet ASIA/ASIA1/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B415A05-045E-284D-9546-D026AE8B2622}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C412B0-2EEC-AC47-91CE-CCCA95D9DD36}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15020" yWindow="10700" windowWidth="12840" windowHeight="10720" xr2:uid="{D26EEBDF-B123-8049-8712-BE9D6DCFC7A4}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <dimension ref="A1:E18322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>